<commit_message>
08/09- Endgame, have added 10-digit codes
</commit_message>
<xml_diff>
--- a/Market_size_factor.xlsx
+++ b/Market_size_factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucar\PycharmProjects\NJORD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucar\PycharmProjects\NJORD_2022_Albin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D587BA6F-319E-47AD-89A9-52792C2241D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DD441E-0685-4816-9F49-A5B710EBFF07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="18384" windowHeight="11580" xr2:uid="{1AF4EA05-DD28-4291-84E3-CA91D8B46552}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1AF4EA05-DD28-4291-84E3-CA91D8B46552}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Market size </t>
   </si>
@@ -51,17 +51,23 @@
     <t>10-100MW</t>
   </si>
   <si>
-    <t>&gt;100 MW</t>
-  </si>
-  <si>
     <t>Factor</t>
+  </si>
+  <si>
+    <t>100-500MW</t>
+  </si>
+  <si>
+    <t>500-1000MW</t>
+  </si>
+  <si>
+    <t>&gt; 1000MW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +80,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -207,17 +219,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BE580A5-0B3B-4694-83C7-6C00BD4D10F2}" name="Tabell20" displayName="Tabell20" ref="A1:F3" totalsRowShown="0" tableBorderDxfId="0">
-  <autoFilter ref="A1:F3" xr:uid="{6BE580A5-0B3B-4694-83C7-6C00BD4D10F2}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BE580A5-0B3B-4694-83C7-6C00BD4D10F2}" name="Tabell20" displayName="Tabell20" ref="A1:H3" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="A1:H3" xr:uid="{6BE580A5-0B3B-4694-83C7-6C00BD4D10F2}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{10933145-D3D0-4F69-B143-0BF8821982FE}" name="Market size "/>
     <tableColumn id="2" xr3:uid="{58DDC71B-90A7-434F-84C0-FEF019DE04EF}" name="0-1MW"/>
     <tableColumn id="3" xr3:uid="{51C68299-8708-4481-8485-F4D85868EEA3}" name="1-5MW"/>
     <tableColumn id="4" xr3:uid="{C4165CFE-85ED-46B4-9947-4E86055A72AF}" name="5-10MW"/>
     <tableColumn id="5" xr3:uid="{9E9F4576-479E-469A-861E-7033777D66DE}" name="10-100MW"/>
-    <tableColumn id="6" xr3:uid="{88F9B78F-FF64-4AA2-BFE8-871765595ED0}" name="&gt;100 MW">
+    <tableColumn id="6" xr3:uid="{88F9B78F-FF64-4AA2-BFE8-871765595ED0}" name="100-500MW">
       <calculatedColumnFormula>0.88709*#REF!</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="7" xr3:uid="{2CCD1583-DFAC-48BE-BB37-0C853314AB0C}" name="500-1000MW"/>
+    <tableColumn id="8" xr3:uid="{B30190C0-6DBF-4693-874A-9CB1907ADBBF}" name="&gt; 1000MW"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -520,15 +534,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D685BF-A383-4820-94C7-1331576058CE}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,12 +559,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="1">
         <f>1.9838*B3</f>
@@ -572,8 +592,16 @@
         <f>0.88709*F3</f>
         <v>1.0201534999999999</v>
       </c>
+      <c r="G2" s="1">
+        <f>1.9838*G3</f>
+        <v>1.38866</v>
+      </c>
+      <c r="H2" s="1">
+        <f>1.79032*H3</f>
+        <v>0.89515999999999996</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1">
         <f>1</f>
@@ -593,8 +621,15 @@
       <c r="F3" s="1">
         <v>1.1499999999999999</v>
       </c>
+      <c r="G3">
+        <v>0.7</v>
+      </c>
+      <c r="H3">
+        <v>0.5</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>